<commit_message>
RDM-3940 Functional tests - label, hint text and displayContext
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v04.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v04.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalkalita/dev/moj/ccd-case-management-web/test/resources/definitionsFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133D8027-1EA3-F244-A233-9D2454932224}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681676D7-6754-4F47-94B5-747D4194E9E2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10880" yWindow="-20800" windowWidth="35820" windowHeight="18140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1863" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1865" uniqueCount="476">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1543,6 +1543,12 @@
   </si>
   <si>
     <t>MySchool.Class.ClassMembers.Children.IsAutistic="Yes"</t>
+  </si>
+  <si>
+    <t>Child full name (UPDATED)</t>
+  </si>
+  <si>
+    <t>Child hint (UPDATED)</t>
   </si>
 </sst>
 </file>
@@ -6841,7 +6847,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8728,7 +8734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -16987,7 +16993,7 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17812,14 +17818,14 @@
         <v>297</v>
       </c>
       <c r="D25" s="57" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="E25" s="57" t="s">
-        <v>442</v>
+        <v>52</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="57" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="7"/>
@@ -17844,14 +17850,14 @@
         <v>297</v>
       </c>
       <c r="D26" s="57" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="E26" s="57" t="s">
-        <v>52</v>
+        <v>442</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="57" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="7"/>
@@ -18200,7 +18206,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18211,7 +18217,7 @@
     <col min="4" max="4" width="23.5" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="57.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
@@ -18329,6 +18335,9 @@
       <c r="F4" s="84" t="s">
         <v>12</v>
       </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
       <c r="J4" s="84" t="s">
         <v>441</v>
       </c>
@@ -18349,6 +18358,9 @@
       <c r="F5" s="84" t="s">
         <v>447</v>
       </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
       <c r="J5" s="84" t="s">
         <v>441</v>
       </c>
@@ -18369,6 +18381,9 @@
       <c r="F6" s="84" t="s">
         <v>464</v>
       </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
       <c r="J6" s="84" t="s">
         <v>441</v>
       </c>
@@ -18389,6 +18404,9 @@
       <c r="F7" s="84" t="s">
         <v>465</v>
       </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
       <c r="J7" s="84" t="s">
         <v>438</v>
       </c>
@@ -18410,13 +18428,19 @@
         <v>456</v>
       </c>
       <c r="F8" s="84" t="s">
-        <v>466</v>
+        <v>467</v>
+      </c>
+      <c r="G8" s="84" t="s">
+        <v>474</v>
+      </c>
+      <c r="H8" s="84" t="s">
+        <v>475</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
       </c>
       <c r="J8" s="84" t="s">
-        <v>438</v>
-      </c>
-      <c r="K8" s="84" t="s">
-        <v>473</v>
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
@@ -18433,7 +18457,10 @@
         <v>456</v>
       </c>
       <c r="F9" s="84" t="s">
-        <v>467</v>
+        <v>468</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
       </c>
       <c r="J9" s="84" t="s">
         <v>441</v>
@@ -18453,10 +18480,13 @@
         <v>456</v>
       </c>
       <c r="F10" s="84" t="s">
-        <v>468</v>
+        <v>469</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
       </c>
       <c r="J10" s="84" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
@@ -18473,10 +18503,16 @@
         <v>456</v>
       </c>
       <c r="F11" s="84" t="s">
-        <v>469</v>
+        <v>470</v>
+      </c>
+      <c r="I11">
+        <v>8</v>
       </c>
       <c r="J11" s="84" t="s">
         <v>438</v>
+      </c>
+      <c r="K11" s="84" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
@@ -18493,17 +18529,18 @@
         <v>456</v>
       </c>
       <c r="F12" s="84" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="J12" s="84" t="s">
         <v>438</v>
       </c>
       <c r="K12" s="84" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>